<commit_message>
Update of import files : the import is now working
</commit_message>
<xml_diff>
--- a/app/code/data/copy_expenses.xlsx
+++ b/app/code/data/copy_expenses.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J402"/>
+  <dimension ref="A1:J385"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15321,652 +15321,6 @@
         </is>
       </c>
     </row>
-    <row r="386">
-      <c r="A386" s="1" t="n">
-        <v>561</v>
-      </c>
-      <c r="B386" t="n">
-        <v>20.49</v>
-      </c>
-      <c r="C386" t="n">
-        <v>562</v>
-      </c>
-      <c r="D386" t="inlineStr"/>
-      <c r="E386" t="inlineStr"/>
-      <c r="F386" t="inlineStr">
-        <is>
-          <t>2020-08-03</t>
-        </is>
-      </c>
-      <c r="G386" t="inlineStr">
-        <is>
-          <t>alimentaire</t>
-        </is>
-      </c>
-      <c r="H386" t="inlineStr">
-        <is>
-          <t>course</t>
-        </is>
-      </c>
-      <c r="I386" t="inlineStr">
-        <is>
-          <t>le crac</t>
-        </is>
-      </c>
-      <c r="J386" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> flocon d avoinne, papaye + mangue sechee</t>
-        </is>
-      </c>
-    </row>
-    <row r="387">
-      <c r="A387" s="1" t="n">
-        <v>562</v>
-      </c>
-      <c r="B387" t="n">
-        <v>26.37</v>
-      </c>
-      <c r="C387" t="n">
-        <v>563</v>
-      </c>
-      <c r="D387" t="inlineStr"/>
-      <c r="E387" t="inlineStr"/>
-      <c r="F387" t="inlineStr">
-        <is>
-          <t>2020-08-03</t>
-        </is>
-      </c>
-      <c r="G387" t="inlineStr">
-        <is>
-          <t>alimentaire</t>
-        </is>
-      </c>
-      <c r="H387" t="inlineStr">
-        <is>
-          <t>course</t>
-        </is>
-      </c>
-      <c r="I387" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J387" t="inlineStr">
-        <is>
-          <t>epicerie europeenne</t>
-        </is>
-      </c>
-    </row>
-    <row r="388">
-      <c r="A388" s="1" t="n">
-        <v>563</v>
-      </c>
-      <c r="B388" t="n">
-        <v>6.67</v>
-      </c>
-      <c r="C388" t="n">
-        <v>564</v>
-      </c>
-      <c r="D388" t="inlineStr"/>
-      <c r="E388" t="inlineStr"/>
-      <c r="F388" t="inlineStr">
-        <is>
-          <t>2020-08-03</t>
-        </is>
-      </c>
-      <c r="G388" t="inlineStr">
-        <is>
-          <t>logement</t>
-        </is>
-      </c>
-      <c r="H388" t="inlineStr">
-        <is>
-          <t>lessive</t>
-        </is>
-      </c>
-      <c r="I388" t="inlineStr">
-        <is>
-          <t>coinomatic</t>
-        </is>
-      </c>
-      <c r="J388" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> argent pour machine a laver</t>
-        </is>
-      </c>
-    </row>
-    <row r="389">
-      <c r="A389" s="1" t="n">
-        <v>565</v>
-      </c>
-      <c r="B389" t="n">
-        <v>6.67</v>
-      </c>
-      <c r="C389" t="n">
-        <v>566</v>
-      </c>
-      <c r="D389" t="inlineStr"/>
-      <c r="E389" t="inlineStr"/>
-      <c r="F389" t="inlineStr">
-        <is>
-          <t>2020-08-07</t>
-        </is>
-      </c>
-      <c r="G389" t="inlineStr">
-        <is>
-          <t>loisir</t>
-        </is>
-      </c>
-      <c r="H389" t="inlineStr">
-        <is>
-          <t>streaming</t>
-        </is>
-      </c>
-      <c r="I389" t="inlineStr">
-        <is>
-          <t>netflix</t>
-        </is>
-      </c>
-      <c r="J389" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> abonnement</t>
-        </is>
-      </c>
-    </row>
-    <row r="390">
-      <c r="A390" s="1" t="n">
-        <v>567</v>
-      </c>
-      <c r="B390" t="n">
-        <v>45.49</v>
-      </c>
-      <c r="C390" t="n">
-        <v>568</v>
-      </c>
-      <c r="D390" t="inlineStr"/>
-      <c r="E390" t="inlineStr"/>
-      <c r="F390" t="inlineStr">
-        <is>
-          <t>2020-08-08</t>
-        </is>
-      </c>
-      <c r="G390" t="inlineStr">
-        <is>
-          <t>alimentaire</t>
-        </is>
-      </c>
-      <c r="H390" t="inlineStr">
-        <is>
-          <t>course</t>
-        </is>
-      </c>
-      <c r="I390" t="inlineStr">
-        <is>
-          <t>provigo</t>
-        </is>
-      </c>
-      <c r="J390" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> courses</t>
-        </is>
-      </c>
-    </row>
-    <row r="391">
-      <c r="A391" s="1" t="n">
-        <v>569</v>
-      </c>
-      <c r="B391" t="n">
-        <v>200</v>
-      </c>
-      <c r="C391" t="n">
-        <v>570</v>
-      </c>
-      <c r="D391" t="inlineStr"/>
-      <c r="E391" t="inlineStr"/>
-      <c r="F391" t="inlineStr">
-        <is>
-          <t>2020-08-09</t>
-        </is>
-      </c>
-      <c r="G391" t="inlineStr">
-        <is>
-          <t>sante</t>
-        </is>
-      </c>
-      <c r="H391" t="inlineStr">
-        <is>
-          <t>medecin</t>
-        </is>
-      </c>
-      <c r="I391" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J391" t="inlineStr">
-        <is>
-          <t>medecin generaliste</t>
-        </is>
-      </c>
-    </row>
-    <row r="392">
-      <c r="A392" s="1" t="n">
-        <v>571</v>
-      </c>
-      <c r="B392" t="n">
-        <v>13.48</v>
-      </c>
-      <c r="C392" t="n">
-        <v>572</v>
-      </c>
-      <c r="D392" t="inlineStr"/>
-      <c r="E392" t="inlineStr"/>
-      <c r="F392" t="inlineStr">
-        <is>
-          <t>2020-08-11</t>
-        </is>
-      </c>
-      <c r="G392" t="inlineStr">
-        <is>
-          <t>alimentaire</t>
-        </is>
-      </c>
-      <c r="H392" t="inlineStr">
-        <is>
-          <t>course</t>
-        </is>
-      </c>
-      <c r="I392" t="inlineStr">
-        <is>
-          <t>provigo</t>
-        </is>
-      </c>
-      <c r="J392" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> courses</t>
-        </is>
-      </c>
-    </row>
-    <row r="393">
-      <c r="A393" s="1" t="n">
-        <v>573</v>
-      </c>
-      <c r="B393" t="n">
-        <v>27.19</v>
-      </c>
-      <c r="C393" t="n">
-        <v>574</v>
-      </c>
-      <c r="D393" t="inlineStr"/>
-      <c r="E393" t="inlineStr"/>
-      <c r="F393" t="inlineStr">
-        <is>
-          <t>2020-08-14</t>
-        </is>
-      </c>
-      <c r="G393" t="inlineStr">
-        <is>
-          <t>alimentaire</t>
-        </is>
-      </c>
-      <c r="H393" t="inlineStr">
-        <is>
-          <t>course</t>
-        </is>
-      </c>
-      <c r="I393" t="inlineStr">
-        <is>
-          <t>provigo</t>
-        </is>
-      </c>
-      <c r="J393" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> courses</t>
-        </is>
-      </c>
-    </row>
-    <row r="394">
-      <c r="A394" s="1" t="n">
-        <v>575</v>
-      </c>
-      <c r="B394" t="n">
-        <v>5.97</v>
-      </c>
-      <c r="C394" t="n">
-        <v>576</v>
-      </c>
-      <c r="D394" t="inlineStr"/>
-      <c r="E394" t="inlineStr"/>
-      <c r="F394" t="inlineStr">
-        <is>
-          <t>2020-08-16</t>
-        </is>
-      </c>
-      <c r="G394" t="inlineStr">
-        <is>
-          <t>alimentaire</t>
-        </is>
-      </c>
-      <c r="H394" t="inlineStr">
-        <is>
-          <t>gourmandise</t>
-        </is>
-      </c>
-      <c r="I394" t="inlineStr">
-        <is>
-          <t>tim horton</t>
-        </is>
-      </c>
-      <c r="J394" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> donuts</t>
-        </is>
-      </c>
-    </row>
-    <row r="395">
-      <c r="A395" s="1" t="n">
-        <v>576</v>
-      </c>
-      <c r="B395" t="n">
-        <v>23.23</v>
-      </c>
-      <c r="C395" t="n">
-        <v>577</v>
-      </c>
-      <c r="D395" t="inlineStr"/>
-      <c r="E395" t="inlineStr"/>
-      <c r="F395" t="inlineStr">
-        <is>
-          <t>2020-08-16</t>
-        </is>
-      </c>
-      <c r="G395" t="inlineStr">
-        <is>
-          <t>alimentaire</t>
-        </is>
-      </c>
-      <c r="H395" t="inlineStr">
-        <is>
-          <t>course</t>
-        </is>
-      </c>
-      <c r="I395" t="inlineStr">
-        <is>
-          <t>metro</t>
-        </is>
-      </c>
-      <c r="J395" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> courses</t>
-        </is>
-      </c>
-    </row>
-    <row r="396">
-      <c r="A396" s="1" t="n">
-        <v>578</v>
-      </c>
-      <c r="B396" t="n">
-        <v>56.67</v>
-      </c>
-      <c r="C396" t="n">
-        <v>579</v>
-      </c>
-      <c r="D396" t="inlineStr"/>
-      <c r="E396" t="inlineStr"/>
-      <c r="F396" t="inlineStr">
-        <is>
-          <t>2020-08-18</t>
-        </is>
-      </c>
-      <c r="G396" t="inlineStr">
-        <is>
-          <t>sante</t>
-        </is>
-      </c>
-      <c r="H396" t="inlineStr">
-        <is>
-          <t>medecin</t>
-        </is>
-      </c>
-      <c r="I396" t="inlineStr">
-        <is>
-          <t>peps</t>
-        </is>
-      </c>
-      <c r="J396" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> kine</t>
-        </is>
-      </c>
-    </row>
-    <row r="397">
-      <c r="A397" s="1" t="n">
-        <v>580</v>
-      </c>
-      <c r="B397" t="n">
-        <v>32.54</v>
-      </c>
-      <c r="C397" t="n">
-        <v>581</v>
-      </c>
-      <c r="D397" t="inlineStr"/>
-      <c r="E397" t="inlineStr"/>
-      <c r="F397" t="inlineStr">
-        <is>
-          <t>2020-08-20</t>
-        </is>
-      </c>
-      <c r="G397" t="inlineStr">
-        <is>
-          <t>alimentaire</t>
-        </is>
-      </c>
-      <c r="H397" t="inlineStr">
-        <is>
-          <t>course</t>
-        </is>
-      </c>
-      <c r="I397" t="inlineStr">
-        <is>
-          <t>provigo</t>
-        </is>
-      </c>
-      <c r="J397" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> courses</t>
-        </is>
-      </c>
-    </row>
-    <row r="398">
-      <c r="A398" s="1" t="n">
-        <v>581</v>
-      </c>
-      <c r="B398" t="n">
-        <v>5.62</v>
-      </c>
-      <c r="C398" t="n">
-        <v>582</v>
-      </c>
-      <c r="D398" t="inlineStr"/>
-      <c r="E398" t="inlineStr"/>
-      <c r="F398" t="inlineStr">
-        <is>
-          <t>2020-08-20</t>
-        </is>
-      </c>
-      <c r="G398" t="inlineStr">
-        <is>
-          <t>alimentaire</t>
-        </is>
-      </c>
-      <c r="H398" t="inlineStr">
-        <is>
-          <t>course</t>
-        </is>
-      </c>
-      <c r="I398" t="inlineStr">
-        <is>
-          <t>metro</t>
-        </is>
-      </c>
-      <c r="J398" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> courses</t>
-        </is>
-      </c>
-    </row>
-    <row r="399">
-      <c r="A399" s="1" t="n">
-        <v>582</v>
-      </c>
-      <c r="B399" t="n">
-        <v>13.43</v>
-      </c>
-      <c r="C399" t="n">
-        <v>583</v>
-      </c>
-      <c r="D399" t="inlineStr"/>
-      <c r="E399" t="inlineStr"/>
-      <c r="F399" t="inlineStr">
-        <is>
-          <t>2020-08-22</t>
-        </is>
-      </c>
-      <c r="G399" t="inlineStr">
-        <is>
-          <t>loisir</t>
-        </is>
-      </c>
-      <c r="H399" t="inlineStr">
-        <is>
-          <t>sortie</t>
-        </is>
-      </c>
-      <c r="I399" t="inlineStr">
-        <is>
-          <t>lvlop</t>
-        </is>
-      </c>
-      <c r="J399" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> aprem gaming</t>
-        </is>
-      </c>
-    </row>
-    <row r="400">
-      <c r="A400" s="1" t="n">
-        <v>585</v>
-      </c>
-      <c r="B400" t="n">
-        <v>14.57</v>
-      </c>
-      <c r="C400" t="n">
-        <v>586</v>
-      </c>
-      <c r="D400" t="inlineStr"/>
-      <c r="E400" t="inlineStr"/>
-      <c r="F400" t="inlineStr">
-        <is>
-          <t>2020-08-25</t>
-        </is>
-      </c>
-      <c r="G400" t="inlineStr">
-        <is>
-          <t>alimentaire</t>
-        </is>
-      </c>
-      <c r="H400" t="inlineStr">
-        <is>
-          <t>restaurant</t>
-        </is>
-      </c>
-      <c r="I400" t="inlineStr">
-        <is>
-          <t>shogun sushi</t>
-        </is>
-      </c>
-      <c r="J400" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> restaurant</t>
-        </is>
-      </c>
-    </row>
-    <row r="401">
-      <c r="A401" s="1" t="n">
-        <v>586</v>
-      </c>
-      <c r="B401" t="n">
-        <v>4.67</v>
-      </c>
-      <c r="C401" t="n">
-        <v>587</v>
-      </c>
-      <c r="D401" t="inlineStr"/>
-      <c r="E401" t="inlineStr"/>
-      <c r="F401" t="inlineStr">
-        <is>
-          <t>2020-08-25</t>
-        </is>
-      </c>
-      <c r="G401" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H401" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I401" t="inlineStr">
-        <is>
-          <t xml:space="preserve">cafe </t>
-        </is>
-      </c>
-      <c r="J401" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="402">
-      <c r="A402" s="1" t="n">
-        <v>587</v>
-      </c>
-      <c r="B402" t="n">
-        <v>8.27</v>
-      </c>
-      <c r="C402" t="n">
-        <v>588</v>
-      </c>
-      <c r="D402" t="inlineStr"/>
-      <c r="E402" t="inlineStr"/>
-      <c r="F402" t="inlineStr">
-        <is>
-          <t>2020-08-26</t>
-        </is>
-      </c>
-      <c r="G402" t="inlineStr">
-        <is>
-          <t>transport</t>
-        </is>
-      </c>
-      <c r="H402" t="inlineStr">
-        <is>
-          <t>bus</t>
-        </is>
-      </c>
-      <c r="I402" t="inlineStr">
-        <is>
-          <t>rtc</t>
-        </is>
-      </c>
-      <c r="J402" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> ticket pour le bus</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>